<commit_message>
Avances 30 de octubre de 2017, parte 4
</commit_message>
<xml_diff>
--- a/img_ejemplos/asteriscos.xlsx
+++ b/img_ejemplos/asteriscos.xlsx
@@ -116,10 +116,10 @@
     <t>EMG</t>
   </si>
   <si>
+    <t>***</t>
+  </si>
+  <si>
     <t>**</t>
-  </si>
-  <si>
-    <t>***</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -226,10 +226,10 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -238,10 +238,10 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
         <v>36</v>
@@ -250,10 +250,10 @@
         <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -261,13 +261,13 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -279,7 +279,7 @@
         <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
         <v>37</v>
@@ -291,10 +291,10 @@
         <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
@@ -302,7 +302,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>36</v>
@@ -332,10 +332,10 @@
         <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -349,34 +349,34 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>36</v>
-      </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -390,10 +390,10 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>36</v>
@@ -414,10 +414,10 @@
         <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">
@@ -425,16 +425,16 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -446,7 +446,7 @@
         <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
         <v>36</v>
@@ -455,10 +455,10 @@
         <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +466,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -475,7 +475,7 @@
         <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
@@ -484,10 +484,10 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
         <v>36</v>
@@ -496,10 +496,10 @@
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
@@ -507,13 +507,13 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
@@ -522,13 +522,13 @@
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
         <v>36</v>
@@ -537,7 +537,7 @@
         <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" t="s">
         <v>36</v>
@@ -548,23 +548,23 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
       <c r="H10" t="s">
         <v>36</v>
       </c>
@@ -578,10 +578,10 @@
         <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
@@ -589,7 +589,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -598,7 +598,7 @@
         <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
         <v>36</v>
@@ -607,7 +607,7 @@
         <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
         <v>37</v>
@@ -619,10 +619,10 @@
         <v>36</v>
       </c>
       <c r="L11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -630,26 +630,26 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
         <v>35</v>
       </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" t="s">
-        <v>37</v>
-      </c>
       <c r="I12" t="s">
         <v>36</v>
       </c>
@@ -660,7 +660,7 @@
         <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M12" t="s">
         <v>36</v>
@@ -677,10 +677,10 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
         <v>36</v>
@@ -689,7 +689,7 @@
         <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" t="s">
         <v>36</v>
@@ -701,10 +701,10 @@
         <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
@@ -718,10 +718,10 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
         <v>36</v>
@@ -730,7 +730,7 @@
         <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
         <v>37</v>
@@ -742,7 +742,7 @@
         <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
         <v>37</v>
@@ -753,16 +753,16 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>36</v>
@@ -780,10 +780,10 @@
         <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M15" t="s">
         <v>37</v>
@@ -794,16 +794,16 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
@@ -812,7 +812,7 @@
         <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
         <v>37</v>
@@ -824,10 +824,10 @@
         <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
@@ -838,10 +838,10 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -853,7 +853,7 @@
         <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" t="s">
         <v>36</v>
@@ -868,7 +868,7 @@
         <v>36</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -882,7 +882,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
         <v>36</v>
@@ -894,7 +894,7 @@
         <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" t="s">
         <v>36</v>
@@ -906,7 +906,7 @@
         <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M18" t="s">
         <v>36</v>
@@ -923,10 +923,10 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F19" t="s">
         <v>36</v>
@@ -935,7 +935,7 @@
         <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
         <v>36</v>
@@ -950,7 +950,7 @@
         <v>36</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -964,7 +964,7 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -976,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I20" t="s">
         <v>36</v>
@@ -988,7 +988,7 @@
         <v>36</v>
       </c>
       <c r="L20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M20" t="s">
         <v>36</v>
@@ -999,37 +999,37 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>37</v>
-      </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" t="s">
         <v>37</v>
       </c>
       <c r="L21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M21" t="s">
         <v>36</v>
@@ -1040,29 +1040,29 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" t="s">
-        <v>37</v>
-      </c>
       <c r="J22" t="s">
         <v>34</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>37</v>
       </c>
       <c r="L22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M22" t="s">
         <v>36</v>
@@ -1081,7 +1081,7 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
@@ -1096,13 +1096,13 @@
         <v>36</v>
       </c>
       <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" t="s">
         <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" t="s">
-        <v>37</v>
       </c>
       <c r="J23" t="s">
         <v>36</v>

</xml_diff>